<commit_message>
redesign sharecode SSIS Package
</commit_message>
<xml_diff>
--- a/MetadataDB_JR/D___Develop/DWReferenceDB_JR.xlsx
+++ b/MetadataDB_JR/D___Develop/DWReferenceDB_JR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7230" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7230" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="SSIS Configuration" sheetId="1" r:id="rId1"/>
@@ -15,16 +15,20 @@
     <sheet name="SaveToDB_LoadedID" sheetId="6" state="veryHidden" r:id="rId6"/>
     <sheet name="SaveToDB_UpdatedID" sheetId="7" state="veryHidden" r:id="rId7"/>
     <sheet name="SaveToDB_Lists" sheetId="8" state="veryHidden" r:id="rId8"/>
+    <sheet name="Suite" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="2" hidden="1">SourceControl!$A$1:$G$3</definedName>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">SourceType!$A$1:$C$6</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'SSIS Configuration'!$A$1:$G$35</definedName>
+    <definedName name="ExternalData_1" localSheetId="8" hidden="1">Suite!$A$1:$I$3</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">SourceControl!$A$1:$G$3</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">SourceType!$A$1:$C$6</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'SSIS Configuration'!$A$1:$G$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">Suite!$A$1:$I$3</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -39,11 +43,14 @@
   <connection id="3" keepAlive="1" name="Connection2" type="5" refreshedVersion="4" savePassword="1" saveData="1">
     <dbPr connection="Provider=SQLOLEDB.1;Integrated Security=SSPI;Persist Security Info=True;Initial Catalog=DWJRReference;Data Source=.;Extended Properties=&quot;&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=4096;Workstation ID=HCMNTB0070;Use Encryption for Data=False;Tag with column collation when possible=False" command="SELECT * FROM [dbo].[SourceControl]"/>
   </connection>
+  <connection id="4" keepAlive="1" name="Connection3" type="5" refreshedVersion="4" savePassword="1" saveData="1">
+    <dbPr connection="Provider=SQLOLEDB.1;Integrated Security=SSPI;Persist Security Info=True;Initial Catalog=DWJRReference;Data Source=.;Extended Properties=&quot;&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=4096;Workstation ID=HCMNTB0070;Use Encryption for Data=False;Tag with column collation when possible=False" command="SELECT [SuiteID], [SuiteName], [Status], [StatusChangeDateTime], DATEADD(DAY, -1, CAST([MaxExpectedExecutionDuration] AS DATETIME)) AS [MaxExpectedExecutionDuration], [MaxExpectedExecutionEmailSent], [SuiteExecutionOrder], [Comments] FROM [dbo].[Suite]"/>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="483">
   <si>
     <t>Use SQL Debug:</t>
   </si>
@@ -1387,6 +1394,111 @@
   </si>
   <si>
     <t>End IDs of object [dbo.SourceControl] on sheet [SourceControl]</t>
+  </si>
+  <si>
+    <t>Start Fields of object [DWJRReference.dbo.Suite] on server [.]</t>
+  </si>
+  <si>
+    <t>SuiteID</t>
+  </si>
+  <si>
+    <t>SuiteName</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>StatusChangeDateTime</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>MaxExpectedExecutionDuration</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>MaxExpectedExecutionEmailSent</t>
+  </si>
+  <si>
+    <t>SuiteExecutionOrder</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>End Fields of object [DWJRReference.dbo.Suite] on server [.]</t>
+  </si>
+  <si>
+    <t>Start User parameter values of object [DWJRReference.dbo.Suite] parameter [SuiteID] on server [.]</t>
+  </si>
+  <si>
+    <t>End User parameter values of object [DWJRReference.dbo.Suite] parameter [SuiteID] on server [.]</t>
+  </si>
+  <si>
+    <t>Start User parameter values of object [DWJRReference.dbo.Suite] parameter [SuiteName] on server [.]</t>
+  </si>
+  <si>
+    <t>End User parameter values of object [DWJRReference.dbo.Suite] parameter [SuiteName] on server [.]</t>
+  </si>
+  <si>
+    <t>Start User parameter values of object [DWJRReference.dbo.Suite] parameter [Status] on server [.]</t>
+  </si>
+  <si>
+    <t>End User parameter values of object [DWJRReference.dbo.Suite] parameter [Status] on server [.]</t>
+  </si>
+  <si>
+    <t>Start User parameter values of object [DWJRReference.dbo.Suite] parameter [StatusChangeDateTime] on server [.]</t>
+  </si>
+  <si>
+    <t>End User parameter values of object [DWJRReference.dbo.Suite] parameter [StatusChangeDateTime] on server [.]</t>
+  </si>
+  <si>
+    <t>Start User parameter values of object [DWJRReference.dbo.Suite] parameter [MaxExpectedExecutionDuration] on server [.]</t>
+  </si>
+  <si>
+    <t>End User parameter values of object [DWJRReference.dbo.Suite] parameter [MaxExpectedExecutionDuration] on server [.]</t>
+  </si>
+  <si>
+    <t>Start User parameter values of object [DWJRReference.dbo.Suite] parameter [MaxExpectedExecutionEmailSent] on server [.]</t>
+  </si>
+  <si>
+    <t>End User parameter values of object [DWJRReference.dbo.Suite] parameter [MaxExpectedExecutionEmailSent] on server [.]</t>
+  </si>
+  <si>
+    <t>Start User parameter values of object [DWJRReference.dbo.Suite] parameter [SuiteExecutionOrder] on server [.]</t>
+  </si>
+  <si>
+    <t>End User parameter values of object [DWJRReference.dbo.Suite] parameter [SuiteExecutionOrder] on server [.]</t>
+  </si>
+  <si>
+    <t>Start User parameter values of object [DWJRReference.dbo.Suite] parameter [Comments] on server [.]</t>
+  </si>
+  <si>
+    <t>End User parameter values of object [DWJRReference.dbo.Suite] parameter [Comments] on server [.]</t>
+  </si>
+  <si>
+    <t>Table_ExternalData_1</t>
+  </si>
+  <si>
+    <t>Start IDs of object [dbo.Suite] on sheet [Suite]</t>
+  </si>
+  <si>
+    <t>End IDs of object [dbo.Suite] on sheet [Suite]</t>
+  </si>
+  <si>
+    <t>FRP</t>
   </si>
 </sst>
 </file>
@@ -1436,17 +1548,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -1467,6 +1581,15 @@
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1522,6 +1645,24 @@
 </queryTable>
 </file>
 
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" rowNumbers="1" backgroundRefresh="0" adjustColumnWidth="0" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh nextId="10">
+    <queryTableFields count="9">
+      <queryTableField id="1" rowNumbers="1" tableColumnId="10"/>
+      <queryTableField id="2" name="SuiteID" tableColumnId="11"/>
+      <queryTableField id="3" name="SuiteName" tableColumnId="12"/>
+      <queryTableField id="4" name="Status" tableColumnId="13"/>
+      <queryTableField id="5" name="StatusChangeDateTime" tableColumnId="14"/>
+      <queryTableField id="6" name="MaxExpectedExecutionDuration" tableColumnId="15"/>
+      <queryTableField id="7" name="MaxExpectedExecutionEmailSent" tableColumnId="16"/>
+      <queryTableField id="8" name="SuiteExecutionOrder" tableColumnId="17"/>
+      <queryTableField id="9" name="Comments" tableColumnId="18"/>
+    </queryTableFields>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Sheet1_Table1" displayName="Sheet1_Table1" ref="A1:G35" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G35"/>
@@ -1561,6 +1702,24 @@
     <tableColumn id="12" uniqueName="12" name="AccessWindowStartMins" queryTableFieldId="5"/>
     <tableColumn id="13" uniqueName="13" name="AccessWindowEndMins" queryTableFieldId="6"/>
     <tableColumn id="14" uniqueName="14" name="SSISConfigurationID" queryTableFieldId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table_ExternalData_1" displayName="Table_ExternalData_1" ref="A1:I3" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:I3"/>
+  <tableColumns count="9">
+    <tableColumn id="10" uniqueName="10" name="_RowNum" queryTableFieldId="1"/>
+    <tableColumn id="11" uniqueName="11" name="SuiteID" queryTableFieldId="2"/>
+    <tableColumn id="12" uniqueName="12" name="SuiteName" queryTableFieldId="3"/>
+    <tableColumn id="13" uniqueName="13" name="Status" queryTableFieldId="4"/>
+    <tableColumn id="14" uniqueName="14" name="StatusChangeDateTime" queryTableFieldId="5" dataDxfId="5"/>
+    <tableColumn id="15" uniqueName="15" name="MaxExpectedExecutionDuration" queryTableFieldId="6" dataDxfId="4"/>
+    <tableColumn id="16" uniqueName="16" name="MaxExpectedExecutionEmailSent" queryTableFieldId="7" dataDxfId="3"/>
+    <tableColumn id="17" uniqueName="17" name="SuiteExecutionOrder" queryTableFieldId="8"/>
+    <tableColumn id="18" uniqueName="18" name="Comments" queryTableFieldId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2775,7 +2934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -2952,7 +3111,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N230"/>
+  <dimension ref="A1:N289"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
@@ -3629,1009 +3788,581 @@
         <v>439</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D107" t="s">
+        <v>449</v>
+      </c>
+      <c r="E107" t="s">
+        <v>11</v>
+      </c>
+      <c r="G107" t="s">
+        <v>12</v>
+      </c>
+      <c r="H107" t="s">
+        <v>13</v>
+      </c>
+      <c r="I107" t="s">
+        <v>14</v>
+      </c>
+      <c r="J107" t="s">
+        <v>15</v>
+      </c>
+      <c r="L107" t="s">
+        <v>16</v>
+      </c>
+      <c r="M107" t="s">
+        <v>14</v>
+      </c>
+      <c r="N107" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D108" t="s">
+        <v>450</v>
+      </c>
+      <c r="E108" t="s">
+        <v>19</v>
+      </c>
+      <c r="G108" t="s">
+        <v>17</v>
+      </c>
+      <c r="H108" t="s">
+        <v>20</v>
+      </c>
+      <c r="I108" t="s">
+        <v>14</v>
+      </c>
+      <c r="J108" t="s">
+        <v>410</v>
+      </c>
+      <c r="K108" t="s">
+        <v>339</v>
+      </c>
+      <c r="N108" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D109" t="s">
+        <v>451</v>
+      </c>
+      <c r="E109" t="s">
+        <v>24</v>
+      </c>
+      <c r="G109" t="s">
+        <v>17</v>
+      </c>
+      <c r="H109" t="s">
+        <v>20</v>
+      </c>
+      <c r="I109" t="s">
+        <v>14</v>
+      </c>
+      <c r="J109" t="s">
+        <v>452</v>
+      </c>
+      <c r="K109" t="s">
+        <v>11</v>
+      </c>
+      <c r="N109" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D110" t="s">
+        <v>453</v>
+      </c>
+      <c r="E110" t="s">
+        <v>27</v>
+      </c>
+      <c r="G110" t="s">
+        <v>17</v>
+      </c>
+      <c r="H110" t="s">
+        <v>20</v>
+      </c>
+      <c r="I110" t="s">
+        <v>14</v>
+      </c>
+      <c r="J110" t="s">
+        <v>454</v>
+      </c>
+      <c r="L110" t="s">
+        <v>24</v>
+      </c>
+      <c r="N110" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D111" t="s">
+        <v>455</v>
+      </c>
+      <c r="E111" t="s">
+        <v>29</v>
+      </c>
+      <c r="G111" t="s">
+        <v>17</v>
+      </c>
+      <c r="H111" t="s">
+        <v>20</v>
+      </c>
+      <c r="I111" t="s">
+        <v>14</v>
+      </c>
+      <c r="J111" t="s">
+        <v>456</v>
+      </c>
+      <c r="L111" t="s">
+        <v>14</v>
+      </c>
+      <c r="N111" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D112" t="s">
+        <v>457</v>
+      </c>
+      <c r="E112" t="s">
+        <v>32</v>
+      </c>
+      <c r="G112" t="s">
+        <v>17</v>
+      </c>
+      <c r="H112" t="s">
+        <v>20</v>
+      </c>
+      <c r="I112" t="s">
+        <v>14</v>
+      </c>
+      <c r="J112" t="s">
+        <v>454</v>
+      </c>
+      <c r="L112" t="s">
+        <v>24</v>
+      </c>
+      <c r="N112" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D113" t="s">
+        <v>458</v>
+      </c>
+      <c r="E113" t="s">
+        <v>459</v>
+      </c>
+      <c r="G113" t="s">
+        <v>17</v>
+      </c>
+      <c r="H113" t="s">
+        <v>20</v>
+      </c>
+      <c r="I113" t="s">
+        <v>14</v>
+      </c>
+      <c r="J113" t="s">
+        <v>15</v>
+      </c>
+      <c r="L113" t="s">
+        <v>16</v>
+      </c>
+      <c r="M113" t="s">
+        <v>14</v>
+      </c>
+      <c r="N113" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D114" t="s">
+        <v>460</v>
+      </c>
+      <c r="E114" t="s">
+        <v>461</v>
+      </c>
+      <c r="G114" t="s">
+        <v>17</v>
+      </c>
+      <c r="H114" t="s">
+        <v>20</v>
+      </c>
+      <c r="I114" t="s">
+        <v>14</v>
+      </c>
+      <c r="J114" t="s">
+        <v>410</v>
+      </c>
+      <c r="K114" t="s">
+        <v>411</v>
+      </c>
+      <c r="N114" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A119" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A120" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A125" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A126" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A161" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A162" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
         <v>49</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B165" t="s">
         <v>13</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D165" t="s">
         <v>50</v>
       </c>
-      <c r="E107" t="s">
+      <c r="E165" t="s">
         <v>51</v>
       </c>
-      <c r="F107" t="s">
+      <c r="F165" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C110" t="s">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C168" t="s">
         <v>55</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D168" t="s">
         <v>56</v>
       </c>
-      <c r="E110" t="s">
+      <c r="E168" t="s">
         <v>57</v>
       </c>
-      <c r="I110" t="s">
+      <c r="I168" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C111" t="s">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C169" t="s">
         <v>55</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D169" t="s">
         <v>59</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E169" t="s">
         <v>57</v>
       </c>
-      <c r="I111" t="s">
+      <c r="I169" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C112" t="s">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C170" t="s">
         <v>55</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D170" t="s">
         <v>61</v>
       </c>
-      <c r="E112" t="s">
+      <c r="E170" t="s">
         <v>57</v>
       </c>
-      <c r="I112" t="s">
+      <c r="I170" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="113" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C113" t="s">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C171" t="s">
         <v>55</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D171" t="s">
         <v>63</v>
       </c>
-      <c r="E113" t="s">
-        <v>64</v>
-      </c>
-      <c r="I113" t="s">
+      <c r="E171" t="s">
+        <v>64</v>
+      </c>
+      <c r="I171" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="114" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C114" t="s">
-        <v>66</v>
-      </c>
-      <c r="D114" t="s">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C172" t="s">
+        <v>66</v>
+      </c>
+      <c r="D172" t="s">
         <v>67</v>
       </c>
-      <c r="E114" t="s">
-        <v>64</v>
-      </c>
-      <c r="I114" t="s">
+      <c r="E172" t="s">
+        <v>64</v>
+      </c>
+      <c r="I172" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="115" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C115" t="s">
-        <v>66</v>
-      </c>
-      <c r="D115" t="s">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C173" t="s">
+        <v>66</v>
+      </c>
+      <c r="D173" t="s">
         <v>69</v>
       </c>
-      <c r="E115" t="s">
+      <c r="E173" t="s">
         <v>57</v>
       </c>
-      <c r="I115" t="s">
+      <c r="I173" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="116" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C116" t="s">
-        <v>66</v>
-      </c>
-      <c r="D116" t="s">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C174" t="s">
+        <v>66</v>
+      </c>
+      <c r="D174" t="s">
         <v>71</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E174" t="s">
         <v>57</v>
       </c>
-      <c r="I116" t="s">
+      <c r="I174" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="117" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C117" t="s">
-        <v>66</v>
-      </c>
-      <c r="D117" t="s">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C175" t="s">
+        <v>66</v>
+      </c>
+      <c r="D175" t="s">
         <v>73</v>
       </c>
-      <c r="E117" t="s">
+      <c r="E175" t="s">
         <v>57</v>
       </c>
-      <c r="I117" t="s">
+      <c r="I175" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="118" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C118" t="s">
-        <v>66</v>
-      </c>
-      <c r="D118" t="s">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C176" t="s">
+        <v>66</v>
+      </c>
+      <c r="D176" t="s">
         <v>75</v>
       </c>
-      <c r="E118" t="s">
+      <c r="E176" t="s">
         <v>57</v>
       </c>
-      <c r="I118" t="s">
+      <c r="I176" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="119" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C119" t="s">
-        <v>66</v>
-      </c>
-      <c r="D119" t="s">
-        <v>77</v>
-      </c>
-      <c r="E119" t="s">
-        <v>57</v>
-      </c>
-      <c r="I119" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="120" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C120" t="s">
-        <v>66</v>
-      </c>
-      <c r="D120" t="s">
-        <v>79</v>
-      </c>
-      <c r="E120" t="s">
-        <v>57</v>
-      </c>
-      <c r="I120" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="121" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C121" t="s">
-        <v>66</v>
-      </c>
-      <c r="D121" t="s">
-        <v>81</v>
-      </c>
-      <c r="E121" t="s">
-        <v>57</v>
-      </c>
-      <c r="I121" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="122" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C122" t="s">
-        <v>66</v>
-      </c>
-      <c r="D122" t="s">
-        <v>83</v>
-      </c>
-      <c r="E122" t="s">
-        <v>64</v>
-      </c>
-      <c r="I122" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="123" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C123" t="s">
-        <v>66</v>
-      </c>
-      <c r="D123" t="s">
-        <v>85</v>
-      </c>
-      <c r="E123" t="s">
-        <v>64</v>
-      </c>
-      <c r="I123" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="124" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C124" t="s">
-        <v>66</v>
-      </c>
-      <c r="D124" t="s">
-        <v>87</v>
-      </c>
-      <c r="E124" t="s">
-        <v>57</v>
-      </c>
-      <c r="I124" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="125" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C125" t="s">
-        <v>66</v>
-      </c>
-      <c r="D125" t="s">
-        <v>89</v>
-      </c>
-      <c r="E125" t="s">
-        <v>57</v>
-      </c>
-      <c r="I125" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="126" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C126" t="s">
-        <v>66</v>
-      </c>
-      <c r="D126" t="s">
-        <v>91</v>
-      </c>
-      <c r="E126" t="s">
-        <v>57</v>
-      </c>
-      <c r="I126" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="127" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C127" t="s">
-        <v>66</v>
-      </c>
-      <c r="D127" t="s">
-        <v>93</v>
-      </c>
-      <c r="E127" t="s">
-        <v>57</v>
-      </c>
-      <c r="I127" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="128" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C128" t="s">
-        <v>66</v>
-      </c>
-      <c r="D128" t="s">
-        <v>95</v>
-      </c>
-      <c r="E128" t="s">
-        <v>57</v>
-      </c>
-      <c r="I128" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="129" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C129" t="s">
-        <v>66</v>
-      </c>
-      <c r="D129" t="s">
-        <v>97</v>
-      </c>
-      <c r="E129" t="s">
-        <v>57</v>
-      </c>
-      <c r="I129" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="130" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C130" t="s">
-        <v>66</v>
-      </c>
-      <c r="D130" t="s">
-        <v>99</v>
-      </c>
-      <c r="E130" t="s">
-        <v>57</v>
-      </c>
-      <c r="I130" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="131" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C131" t="s">
-        <v>66</v>
-      </c>
-      <c r="D131" t="s">
-        <v>101</v>
-      </c>
-      <c r="E131" t="s">
-        <v>64</v>
-      </c>
-      <c r="I131" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="132" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C132" t="s">
-        <v>66</v>
-      </c>
-      <c r="D132" t="s">
-        <v>103</v>
-      </c>
-      <c r="E132" t="s">
-        <v>64</v>
-      </c>
-      <c r="I132" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="133" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C133" t="s">
-        <v>66</v>
-      </c>
-      <c r="D133" t="s">
-        <v>105</v>
-      </c>
-      <c r="E133" t="s">
-        <v>64</v>
-      </c>
-      <c r="I133" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="134" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C134" t="s">
-        <v>66</v>
-      </c>
-      <c r="D134" t="s">
-        <v>107</v>
-      </c>
-      <c r="E134" t="s">
-        <v>64</v>
-      </c>
-      <c r="I134" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="135" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C135" t="s">
-        <v>66</v>
-      </c>
-      <c r="D135" t="s">
-        <v>109</v>
-      </c>
-      <c r="E135" t="s">
-        <v>64</v>
-      </c>
-      <c r="I135" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="136" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C136" t="s">
-        <v>66</v>
-      </c>
-      <c r="D136" t="s">
-        <v>111</v>
-      </c>
-      <c r="E136" t="s">
-        <v>64</v>
-      </c>
-      <c r="I136" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="137" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C137" t="s">
-        <v>66</v>
-      </c>
-      <c r="D137" t="s">
-        <v>113</v>
-      </c>
-      <c r="E137" t="s">
-        <v>64</v>
-      </c>
-      <c r="I137" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="138" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C138" t="s">
-        <v>66</v>
-      </c>
-      <c r="D138" t="s">
-        <v>115</v>
-      </c>
-      <c r="E138" t="s">
-        <v>64</v>
-      </c>
-      <c r="I138" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="139" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C139" t="s">
-        <v>66</v>
-      </c>
-      <c r="D139" t="s">
-        <v>117</v>
-      </c>
-      <c r="E139" t="s">
-        <v>64</v>
-      </c>
-      <c r="I139" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="140" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C140" t="s">
-        <v>66</v>
-      </c>
-      <c r="D140" t="s">
-        <v>119</v>
-      </c>
-      <c r="E140" t="s">
-        <v>64</v>
-      </c>
-      <c r="I140" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="141" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C141" t="s">
-        <v>66</v>
-      </c>
-      <c r="D141" t="s">
-        <v>121</v>
-      </c>
-      <c r="E141" t="s">
-        <v>64</v>
-      </c>
-      <c r="I141" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="142" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C142" t="s">
-        <v>66</v>
-      </c>
-      <c r="D142" t="s">
-        <v>123</v>
-      </c>
-      <c r="E142" t="s">
-        <v>64</v>
-      </c>
-      <c r="I142" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="143" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C143" t="s">
-        <v>66</v>
-      </c>
-      <c r="D143" t="s">
-        <v>125</v>
-      </c>
-      <c r="E143" t="s">
-        <v>64</v>
-      </c>
-      <c r="I143" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="144" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C144" t="s">
-        <v>66</v>
-      </c>
-      <c r="D144" t="s">
-        <v>127</v>
-      </c>
-      <c r="E144" t="s">
-        <v>64</v>
-      </c>
-      <c r="I144" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="145" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C145" t="s">
-        <v>66</v>
-      </c>
-      <c r="D145" t="s">
-        <v>129</v>
-      </c>
-      <c r="E145" t="s">
-        <v>64</v>
-      </c>
-      <c r="I145" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="146" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C146" t="s">
-        <v>66</v>
-      </c>
-      <c r="D146" t="s">
-        <v>131</v>
-      </c>
-      <c r="E146" t="s">
-        <v>64</v>
-      </c>
-      <c r="I146" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="147" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C147" t="s">
-        <v>66</v>
-      </c>
-      <c r="D147" t="s">
-        <v>133</v>
-      </c>
-      <c r="E147" t="s">
-        <v>64</v>
-      </c>
-      <c r="I147" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="148" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C148" t="s">
-        <v>66</v>
-      </c>
-      <c r="D148" t="s">
-        <v>135</v>
-      </c>
-      <c r="E148" t="s">
-        <v>64</v>
-      </c>
-      <c r="I148" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="149" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C149" t="s">
-        <v>66</v>
-      </c>
-      <c r="D149" t="s">
-        <v>137</v>
-      </c>
-      <c r="E149" t="s">
-        <v>64</v>
-      </c>
-      <c r="I149" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="150" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C150" t="s">
-        <v>66</v>
-      </c>
-      <c r="D150" t="s">
-        <v>139</v>
-      </c>
-      <c r="E150" t="s">
-        <v>64</v>
-      </c>
-      <c r="I150" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="151" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C151" t="s">
-        <v>66</v>
-      </c>
-      <c r="D151" t="s">
-        <v>141</v>
-      </c>
-      <c r="E151" t="s">
-        <v>64</v>
-      </c>
-      <c r="I151" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="152" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C152" t="s">
-        <v>66</v>
-      </c>
-      <c r="D152" t="s">
-        <v>143</v>
-      </c>
-      <c r="E152" t="s">
-        <v>64</v>
-      </c>
-      <c r="I152" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="153" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C153" t="s">
-        <v>66</v>
-      </c>
-      <c r="D153" t="s">
-        <v>145</v>
-      </c>
-      <c r="E153" t="s">
-        <v>64</v>
-      </c>
-      <c r="I153" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="154" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C154" t="s">
-        <v>66</v>
-      </c>
-      <c r="D154" t="s">
-        <v>147</v>
-      </c>
-      <c r="E154" t="s">
-        <v>64</v>
-      </c>
-      <c r="I154" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="155" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C155" t="s">
-        <v>66</v>
-      </c>
-      <c r="D155" t="s">
-        <v>149</v>
-      </c>
-      <c r="E155" t="s">
-        <v>64</v>
-      </c>
-      <c r="I155" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="156" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C156" t="s">
-        <v>66</v>
-      </c>
-      <c r="D156" t="s">
-        <v>151</v>
-      </c>
-      <c r="E156" t="s">
-        <v>64</v>
-      </c>
-      <c r="I156" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="157" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C157" t="s">
-        <v>66</v>
-      </c>
-      <c r="D157" t="s">
-        <v>153</v>
-      </c>
-      <c r="E157" t="s">
-        <v>64</v>
-      </c>
-      <c r="I157" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="158" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C158" t="s">
-        <v>66</v>
-      </c>
-      <c r="D158" t="s">
-        <v>155</v>
-      </c>
-      <c r="E158" t="s">
-        <v>64</v>
-      </c>
-      <c r="I158" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="159" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C159" t="s">
-        <v>66</v>
-      </c>
-      <c r="D159" t="s">
-        <v>157</v>
-      </c>
-      <c r="E159" t="s">
-        <v>64</v>
-      </c>
-      <c r="I159" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="160" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C160" t="s">
-        <v>66</v>
-      </c>
-      <c r="D160" t="s">
-        <v>159</v>
-      </c>
-      <c r="E160" t="s">
-        <v>64</v>
-      </c>
-      <c r="I160" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="161" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C161" t="s">
-        <v>66</v>
-      </c>
-      <c r="D161" t="s">
-        <v>161</v>
-      </c>
-      <c r="E161" t="s">
-        <v>64</v>
-      </c>
-      <c r="I161" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="162" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C162" t="s">
-        <v>66</v>
-      </c>
-      <c r="D162" t="s">
-        <v>163</v>
-      </c>
-      <c r="E162" t="s">
-        <v>64</v>
-      </c>
-      <c r="I162" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="163" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C163" t="s">
-        <v>66</v>
-      </c>
-      <c r="D163" t="s">
-        <v>165</v>
-      </c>
-      <c r="E163" t="s">
-        <v>64</v>
-      </c>
-      <c r="I163" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="164" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C164" t="s">
-        <v>66</v>
-      </c>
-      <c r="D164" t="s">
-        <v>167</v>
-      </c>
-      <c r="E164" t="s">
-        <v>64</v>
-      </c>
-      <c r="I164" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="165" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C165" t="s">
-        <v>66</v>
-      </c>
-      <c r="D165" t="s">
-        <v>169</v>
-      </c>
-      <c r="E165" t="s">
-        <v>64</v>
-      </c>
-      <c r="I165" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="166" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C166" t="s">
-        <v>66</v>
-      </c>
-      <c r="D166" t="s">
-        <v>171</v>
-      </c>
-      <c r="E166" t="s">
-        <v>64</v>
-      </c>
-      <c r="I166" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="167" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C167" t="s">
-        <v>66</v>
-      </c>
-      <c r="D167" t="s">
-        <v>173</v>
-      </c>
-      <c r="E167" t="s">
-        <v>64</v>
-      </c>
-      <c r="I167" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="168" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C168" t="s">
-        <v>66</v>
-      </c>
-      <c r="D168" t="s">
-        <v>175</v>
-      </c>
-      <c r="E168" t="s">
-        <v>64</v>
-      </c>
-      <c r="I168" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="169" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C169" t="s">
-        <v>66</v>
-      </c>
-      <c r="D169" t="s">
-        <v>177</v>
-      </c>
-      <c r="E169" t="s">
-        <v>64</v>
-      </c>
-      <c r="I169" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="170" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C170" t="s">
-        <v>66</v>
-      </c>
-      <c r="D170" t="s">
-        <v>179</v>
-      </c>
-      <c r="E170" t="s">
-        <v>64</v>
-      </c>
-      <c r="I170" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="171" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C171" t="s">
-        <v>66</v>
-      </c>
-      <c r="D171" t="s">
-        <v>181</v>
-      </c>
-      <c r="E171" t="s">
-        <v>64</v>
-      </c>
-      <c r="I171" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="172" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C172" t="s">
-        <v>66</v>
-      </c>
-      <c r="D172" t="s">
-        <v>183</v>
-      </c>
-      <c r="E172" t="s">
-        <v>64</v>
-      </c>
-      <c r="I172" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="173" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C173" t="s">
-        <v>66</v>
-      </c>
-      <c r="D173" t="s">
-        <v>185</v>
-      </c>
-      <c r="E173" t="s">
-        <v>64</v>
-      </c>
-      <c r="I173" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="174" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C174" t="s">
-        <v>66</v>
-      </c>
-      <c r="D174" t="s">
-        <v>187</v>
-      </c>
-      <c r="E174" t="s">
-        <v>64</v>
-      </c>
-      <c r="I174" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="175" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C175" t="s">
-        <v>66</v>
-      </c>
-      <c r="D175" t="s">
-        <v>189</v>
-      </c>
-      <c r="E175" t="s">
-        <v>64</v>
-      </c>
-      <c r="I175" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="176" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C176" t="s">
-        <v>66</v>
-      </c>
-      <c r="D176" t="s">
-        <v>191</v>
-      </c>
-      <c r="E176" t="s">
-        <v>64</v>
-      </c>
-      <c r="I176" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="177" spans="3:9" x14ac:dyDescent="0.2">
@@ -4639,13 +4370,13 @@
         <v>66</v>
       </c>
       <c r="D177" t="s">
-        <v>193</v>
+        <v>77</v>
       </c>
       <c r="E177" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="I177" t="s">
-        <v>194</v>
+        <v>78</v>
       </c>
     </row>
     <row r="178" spans="3:9" x14ac:dyDescent="0.2">
@@ -4653,13 +4384,13 @@
         <v>66</v>
       </c>
       <c r="D178" t="s">
-        <v>195</v>
+        <v>79</v>
       </c>
       <c r="E178" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="I178" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
     </row>
     <row r="179" spans="3:9" x14ac:dyDescent="0.2">
@@ -4667,13 +4398,13 @@
         <v>66</v>
       </c>
       <c r="D179" t="s">
-        <v>197</v>
+        <v>81</v>
       </c>
       <c r="E179" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="I179" t="s">
-        <v>198</v>
+        <v>82</v>
       </c>
     </row>
     <row r="180" spans="3:9" x14ac:dyDescent="0.2">
@@ -4681,13 +4412,13 @@
         <v>66</v>
       </c>
       <c r="D180" t="s">
-        <v>199</v>
+        <v>83</v>
       </c>
       <c r="E180" t="s">
         <v>64</v>
       </c>
       <c r="I180" t="s">
-        <v>200</v>
+        <v>84</v>
       </c>
     </row>
     <row r="181" spans="3:9" x14ac:dyDescent="0.2">
@@ -4695,13 +4426,13 @@
         <v>66</v>
       </c>
       <c r="D181" t="s">
-        <v>201</v>
+        <v>85</v>
       </c>
       <c r="E181" t="s">
         <v>64</v>
       </c>
       <c r="I181" t="s">
-        <v>202</v>
+        <v>86</v>
       </c>
     </row>
     <row r="182" spans="3:9" x14ac:dyDescent="0.2">
@@ -4709,13 +4440,13 @@
         <v>66</v>
       </c>
       <c r="D182" t="s">
-        <v>203</v>
+        <v>87</v>
       </c>
       <c r="E182" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="I182" t="s">
-        <v>204</v>
+        <v>88</v>
       </c>
     </row>
     <row r="183" spans="3:9" x14ac:dyDescent="0.2">
@@ -4723,13 +4454,13 @@
         <v>66</v>
       </c>
       <c r="D183" t="s">
-        <v>205</v>
+        <v>89</v>
       </c>
       <c r="E183" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="I183" t="s">
-        <v>206</v>
+        <v>90</v>
       </c>
     </row>
     <row r="184" spans="3:9" x14ac:dyDescent="0.2">
@@ -4737,13 +4468,13 @@
         <v>66</v>
       </c>
       <c r="D184" t="s">
-        <v>207</v>
+        <v>91</v>
       </c>
       <c r="E184" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="I184" t="s">
-        <v>208</v>
+        <v>92</v>
       </c>
     </row>
     <row r="185" spans="3:9" x14ac:dyDescent="0.2">
@@ -4751,13 +4482,13 @@
         <v>66</v>
       </c>
       <c r="D185" t="s">
-        <v>209</v>
+        <v>93</v>
       </c>
       <c r="E185" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="I185" t="s">
-        <v>210</v>
+        <v>94</v>
       </c>
     </row>
     <row r="186" spans="3:9" x14ac:dyDescent="0.2">
@@ -4765,13 +4496,13 @@
         <v>66</v>
       </c>
       <c r="D186" t="s">
-        <v>211</v>
+        <v>95</v>
       </c>
       <c r="E186" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="I186" t="s">
-        <v>212</v>
+        <v>96</v>
       </c>
     </row>
     <row r="187" spans="3:9" x14ac:dyDescent="0.2">
@@ -4779,13 +4510,13 @@
         <v>66</v>
       </c>
       <c r="D187" t="s">
-        <v>213</v>
+        <v>97</v>
       </c>
       <c r="E187" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="I187" t="s">
-        <v>214</v>
+        <v>98</v>
       </c>
     </row>
     <row r="188" spans="3:9" x14ac:dyDescent="0.2">
@@ -4793,13 +4524,13 @@
         <v>66</v>
       </c>
       <c r="D188" t="s">
-        <v>215</v>
+        <v>99</v>
       </c>
       <c r="E188" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="I188" t="s">
-        <v>216</v>
+        <v>100</v>
       </c>
     </row>
     <row r="189" spans="3:9" x14ac:dyDescent="0.2">
@@ -4807,13 +4538,13 @@
         <v>66</v>
       </c>
       <c r="D189" t="s">
-        <v>217</v>
+        <v>101</v>
       </c>
       <c r="E189" t="s">
         <v>64</v>
       </c>
       <c r="I189" t="s">
-        <v>218</v>
+        <v>102</v>
       </c>
     </row>
     <row r="190" spans="3:9" x14ac:dyDescent="0.2">
@@ -4821,13 +4552,13 @@
         <v>66</v>
       </c>
       <c r="D190" t="s">
-        <v>219</v>
+        <v>103</v>
       </c>
       <c r="E190" t="s">
         <v>64</v>
       </c>
       <c r="I190" t="s">
-        <v>220</v>
+        <v>104</v>
       </c>
     </row>
     <row r="191" spans="3:9" x14ac:dyDescent="0.2">
@@ -4835,13 +4566,13 @@
         <v>66</v>
       </c>
       <c r="D191" t="s">
-        <v>221</v>
+        <v>105</v>
       </c>
       <c r="E191" t="s">
         <v>64</v>
       </c>
       <c r="I191" t="s">
-        <v>222</v>
+        <v>106</v>
       </c>
     </row>
     <row r="192" spans="3:9" x14ac:dyDescent="0.2">
@@ -4849,13 +4580,13 @@
         <v>66</v>
       </c>
       <c r="D192" t="s">
-        <v>223</v>
+        <v>107</v>
       </c>
       <c r="E192" t="s">
         <v>64</v>
       </c>
       <c r="I192" t="s">
-        <v>224</v>
+        <v>108</v>
       </c>
     </row>
     <row r="193" spans="3:9" x14ac:dyDescent="0.2">
@@ -4863,13 +4594,13 @@
         <v>66</v>
       </c>
       <c r="D193" t="s">
-        <v>225</v>
+        <v>109</v>
       </c>
       <c r="E193" t="s">
         <v>64</v>
       </c>
       <c r="I193" t="s">
-        <v>226</v>
+        <v>110</v>
       </c>
     </row>
     <row r="194" spans="3:9" x14ac:dyDescent="0.2">
@@ -4877,13 +4608,13 @@
         <v>66</v>
       </c>
       <c r="D194" t="s">
-        <v>227</v>
+        <v>111</v>
       </c>
       <c r="E194" t="s">
         <v>64</v>
       </c>
       <c r="I194" t="s">
-        <v>228</v>
+        <v>112</v>
       </c>
     </row>
     <row r="195" spans="3:9" x14ac:dyDescent="0.2">
@@ -4891,13 +4622,13 @@
         <v>66</v>
       </c>
       <c r="D195" t="s">
-        <v>229</v>
+        <v>113</v>
       </c>
       <c r="E195" t="s">
         <v>64</v>
       </c>
       <c r="I195" t="s">
-        <v>230</v>
+        <v>114</v>
       </c>
     </row>
     <row r="196" spans="3:9" x14ac:dyDescent="0.2">
@@ -4905,13 +4636,13 @@
         <v>66</v>
       </c>
       <c r="D196" t="s">
-        <v>231</v>
+        <v>115</v>
       </c>
       <c r="E196" t="s">
         <v>64</v>
       </c>
       <c r="I196" t="s">
-        <v>232</v>
+        <v>116</v>
       </c>
     </row>
     <row r="197" spans="3:9" x14ac:dyDescent="0.2">
@@ -4919,13 +4650,13 @@
         <v>66</v>
       </c>
       <c r="D197" t="s">
-        <v>233</v>
+        <v>117</v>
       </c>
       <c r="E197" t="s">
         <v>64</v>
       </c>
       <c r="I197" t="s">
-        <v>234</v>
+        <v>118</v>
       </c>
     </row>
     <row r="198" spans="3:9" x14ac:dyDescent="0.2">
@@ -4933,13 +4664,13 @@
         <v>66</v>
       </c>
       <c r="D198" t="s">
-        <v>235</v>
+        <v>119</v>
       </c>
       <c r="E198" t="s">
         <v>64</v>
       </c>
       <c r="I198" t="s">
-        <v>236</v>
+        <v>120</v>
       </c>
     </row>
     <row r="199" spans="3:9" x14ac:dyDescent="0.2">
@@ -4947,13 +4678,13 @@
         <v>66</v>
       </c>
       <c r="D199" t="s">
-        <v>237</v>
+        <v>121</v>
       </c>
       <c r="E199" t="s">
         <v>64</v>
       </c>
       <c r="I199" t="s">
-        <v>238</v>
+        <v>122</v>
       </c>
     </row>
     <row r="200" spans="3:9" x14ac:dyDescent="0.2">
@@ -4961,13 +4692,13 @@
         <v>66</v>
       </c>
       <c r="D200" t="s">
-        <v>239</v>
+        <v>123</v>
       </c>
       <c r="E200" t="s">
         <v>64</v>
       </c>
       <c r="I200" t="s">
-        <v>240</v>
+        <v>124</v>
       </c>
     </row>
     <row r="201" spans="3:9" x14ac:dyDescent="0.2">
@@ -4975,13 +4706,13 @@
         <v>66</v>
       </c>
       <c r="D201" t="s">
-        <v>241</v>
+        <v>125</v>
       </c>
       <c r="E201" t="s">
         <v>64</v>
       </c>
       <c r="I201" t="s">
-        <v>242</v>
+        <v>126</v>
       </c>
     </row>
     <row r="202" spans="3:9" x14ac:dyDescent="0.2">
@@ -4989,13 +4720,13 @@
         <v>66</v>
       </c>
       <c r="D202" t="s">
-        <v>243</v>
+        <v>127</v>
       </c>
       <c r="E202" t="s">
         <v>64</v>
       </c>
       <c r="I202" t="s">
-        <v>244</v>
+        <v>128</v>
       </c>
     </row>
     <row r="203" spans="3:9" x14ac:dyDescent="0.2">
@@ -5003,13 +4734,13 @@
         <v>66</v>
       </c>
       <c r="D203" t="s">
-        <v>245</v>
+        <v>129</v>
       </c>
       <c r="E203" t="s">
         <v>64</v>
       </c>
       <c r="I203" t="s">
-        <v>246</v>
+        <v>130</v>
       </c>
     </row>
     <row r="204" spans="3:9" x14ac:dyDescent="0.2">
@@ -5017,13 +4748,13 @@
         <v>66</v>
       </c>
       <c r="D204" t="s">
-        <v>247</v>
+        <v>131</v>
       </c>
       <c r="E204" t="s">
         <v>64</v>
       </c>
       <c r="I204" t="s">
-        <v>248</v>
+        <v>132</v>
       </c>
     </row>
     <row r="205" spans="3:9" x14ac:dyDescent="0.2">
@@ -5031,13 +4762,13 @@
         <v>66</v>
       </c>
       <c r="D205" t="s">
-        <v>249</v>
+        <v>133</v>
       </c>
       <c r="E205" t="s">
         <v>64</v>
       </c>
       <c r="I205" t="s">
-        <v>250</v>
+        <v>134</v>
       </c>
     </row>
     <row r="206" spans="3:9" x14ac:dyDescent="0.2">
@@ -5045,13 +4776,13 @@
         <v>66</v>
       </c>
       <c r="D206" t="s">
-        <v>251</v>
+        <v>135</v>
       </c>
       <c r="E206" t="s">
         <v>64</v>
       </c>
       <c r="I206" t="s">
-        <v>252</v>
+        <v>136</v>
       </c>
     </row>
     <row r="207" spans="3:9" x14ac:dyDescent="0.2">
@@ -5059,13 +4790,13 @@
         <v>66</v>
       </c>
       <c r="D207" t="s">
-        <v>253</v>
+        <v>137</v>
       </c>
       <c r="E207" t="s">
         <v>64</v>
       </c>
       <c r="I207" t="s">
-        <v>254</v>
+        <v>138</v>
       </c>
     </row>
     <row r="208" spans="3:9" x14ac:dyDescent="0.2">
@@ -5073,13 +4804,13 @@
         <v>66</v>
       </c>
       <c r="D208" t="s">
-        <v>255</v>
+        <v>139</v>
       </c>
       <c r="E208" t="s">
         <v>64</v>
       </c>
       <c r="I208" t="s">
-        <v>256</v>
+        <v>140</v>
       </c>
     </row>
     <row r="209" spans="3:9" x14ac:dyDescent="0.2">
@@ -5087,13 +4818,13 @@
         <v>66</v>
       </c>
       <c r="D209" t="s">
-        <v>257</v>
+        <v>141</v>
       </c>
       <c r="E209" t="s">
         <v>64</v>
       </c>
       <c r="I209" t="s">
-        <v>258</v>
+        <v>142</v>
       </c>
     </row>
     <row r="210" spans="3:9" x14ac:dyDescent="0.2">
@@ -5101,13 +4832,13 @@
         <v>66</v>
       </c>
       <c r="D210" t="s">
-        <v>259</v>
+        <v>143</v>
       </c>
       <c r="E210" t="s">
         <v>64</v>
       </c>
       <c r="I210" t="s">
-        <v>260</v>
+        <v>144</v>
       </c>
     </row>
     <row r="211" spans="3:9" x14ac:dyDescent="0.2">
@@ -5115,13 +4846,13 @@
         <v>66</v>
       </c>
       <c r="D211" t="s">
-        <v>261</v>
+        <v>145</v>
       </c>
       <c r="E211" t="s">
         <v>64</v>
       </c>
       <c r="I211" t="s">
-        <v>262</v>
+        <v>146</v>
       </c>
     </row>
     <row r="212" spans="3:9" x14ac:dyDescent="0.2">
@@ -5129,13 +4860,13 @@
         <v>66</v>
       </c>
       <c r="D212" t="s">
-        <v>263</v>
+        <v>147</v>
       </c>
       <c r="E212" t="s">
         <v>64</v>
       </c>
       <c r="I212" t="s">
-        <v>264</v>
+        <v>148</v>
       </c>
     </row>
     <row r="213" spans="3:9" x14ac:dyDescent="0.2">
@@ -5143,13 +4874,13 @@
         <v>66</v>
       </c>
       <c r="D213" t="s">
-        <v>265</v>
+        <v>149</v>
       </c>
       <c r="E213" t="s">
         <v>64</v>
       </c>
       <c r="I213" t="s">
-        <v>266</v>
+        <v>150</v>
       </c>
     </row>
     <row r="214" spans="3:9" x14ac:dyDescent="0.2">
@@ -5157,13 +4888,13 @@
         <v>66</v>
       </c>
       <c r="D214" t="s">
-        <v>267</v>
+        <v>151</v>
       </c>
       <c r="E214" t="s">
         <v>64</v>
       </c>
       <c r="I214" t="s">
-        <v>268</v>
+        <v>152</v>
       </c>
     </row>
     <row r="215" spans="3:9" x14ac:dyDescent="0.2">
@@ -5171,13 +4902,13 @@
         <v>66</v>
       </c>
       <c r="D215" t="s">
-        <v>269</v>
+        <v>153</v>
       </c>
       <c r="E215" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="I215" t="s">
-        <v>270</v>
+        <v>154</v>
       </c>
     </row>
     <row r="216" spans="3:9" x14ac:dyDescent="0.2">
@@ -5185,13 +4916,13 @@
         <v>66</v>
       </c>
       <c r="D216" t="s">
-        <v>271</v>
+        <v>155</v>
       </c>
       <c r="E216" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="I216" t="s">
-        <v>272</v>
+        <v>156</v>
       </c>
     </row>
     <row r="217" spans="3:9" x14ac:dyDescent="0.2">
@@ -5199,13 +4930,13 @@
         <v>66</v>
       </c>
       <c r="D217" t="s">
-        <v>273</v>
+        <v>157</v>
       </c>
       <c r="E217" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="I217" t="s">
-        <v>274</v>
+        <v>158</v>
       </c>
     </row>
     <row r="218" spans="3:9" x14ac:dyDescent="0.2">
@@ -5213,13 +4944,13 @@
         <v>66</v>
       </c>
       <c r="D218" t="s">
-        <v>275</v>
+        <v>159</v>
       </c>
       <c r="E218" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="I218" t="s">
-        <v>276</v>
+        <v>160</v>
       </c>
     </row>
     <row r="219" spans="3:9" x14ac:dyDescent="0.2">
@@ -5227,13 +4958,13 @@
         <v>66</v>
       </c>
       <c r="D219" t="s">
-        <v>277</v>
+        <v>161</v>
       </c>
       <c r="E219" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="I219" t="s">
-        <v>278</v>
+        <v>162</v>
       </c>
     </row>
     <row r="220" spans="3:9" x14ac:dyDescent="0.2">
@@ -5241,13 +4972,13 @@
         <v>66</v>
       </c>
       <c r="D220" t="s">
-        <v>279</v>
+        <v>163</v>
       </c>
       <c r="E220" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="I220" t="s">
-        <v>280</v>
+        <v>164</v>
       </c>
     </row>
     <row r="221" spans="3:9" x14ac:dyDescent="0.2">
@@ -5255,13 +4986,13 @@
         <v>66</v>
       </c>
       <c r="D221" t="s">
-        <v>281</v>
+        <v>165</v>
       </c>
       <c r="E221" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="I221" t="s">
-        <v>282</v>
+        <v>166</v>
       </c>
     </row>
     <row r="222" spans="3:9" x14ac:dyDescent="0.2">
@@ -5269,13 +5000,13 @@
         <v>66</v>
       </c>
       <c r="D222" t="s">
-        <v>283</v>
+        <v>167</v>
       </c>
       <c r="E222" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="I222" t="s">
-        <v>284</v>
+        <v>168</v>
       </c>
     </row>
     <row r="223" spans="3:9" x14ac:dyDescent="0.2">
@@ -5283,13 +5014,13 @@
         <v>66</v>
       </c>
       <c r="D223" t="s">
-        <v>285</v>
+        <v>169</v>
       </c>
       <c r="E223" t="s">
-        <v>286</v>
+        <v>64</v>
       </c>
       <c r="I223" t="s">
-        <v>287</v>
+        <v>170</v>
       </c>
     </row>
     <row r="224" spans="3:9" x14ac:dyDescent="0.2">
@@ -5297,78 +5028,907 @@
         <v>66</v>
       </c>
       <c r="D224" t="s">
+        <v>171</v>
+      </c>
+      <c r="E224" t="s">
+        <v>64</v>
+      </c>
+      <c r="I224" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="225" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C225" t="s">
+        <v>66</v>
+      </c>
+      <c r="D225" t="s">
+        <v>173</v>
+      </c>
+      <c r="E225" t="s">
+        <v>64</v>
+      </c>
+      <c r="I225" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="226" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C226" t="s">
+        <v>66</v>
+      </c>
+      <c r="D226" t="s">
+        <v>175</v>
+      </c>
+      <c r="E226" t="s">
+        <v>64</v>
+      </c>
+      <c r="I226" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="227" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C227" t="s">
+        <v>66</v>
+      </c>
+      <c r="D227" t="s">
+        <v>177</v>
+      </c>
+      <c r="E227" t="s">
+        <v>64</v>
+      </c>
+      <c r="I227" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="228" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C228" t="s">
+        <v>66</v>
+      </c>
+      <c r="D228" t="s">
+        <v>179</v>
+      </c>
+      <c r="E228" t="s">
+        <v>64</v>
+      </c>
+      <c r="I228" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="229" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C229" t="s">
+        <v>66</v>
+      </c>
+      <c r="D229" t="s">
+        <v>181</v>
+      </c>
+      <c r="E229" t="s">
+        <v>64</v>
+      </c>
+      <c r="I229" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="230" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C230" t="s">
+        <v>66</v>
+      </c>
+      <c r="D230" t="s">
+        <v>183</v>
+      </c>
+      <c r="E230" t="s">
+        <v>64</v>
+      </c>
+      <c r="I230" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="231" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C231" t="s">
+        <v>66</v>
+      </c>
+      <c r="D231" t="s">
+        <v>185</v>
+      </c>
+      <c r="E231" t="s">
+        <v>64</v>
+      </c>
+      <c r="I231" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="232" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C232" t="s">
+        <v>66</v>
+      </c>
+      <c r="D232" t="s">
+        <v>187</v>
+      </c>
+      <c r="E232" t="s">
+        <v>64</v>
+      </c>
+      <c r="I232" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="233" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C233" t="s">
+        <v>66</v>
+      </c>
+      <c r="D233" t="s">
+        <v>189</v>
+      </c>
+      <c r="E233" t="s">
+        <v>64</v>
+      </c>
+      <c r="I233" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="234" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C234" t="s">
+        <v>66</v>
+      </c>
+      <c r="D234" t="s">
+        <v>191</v>
+      </c>
+      <c r="E234" t="s">
+        <v>64</v>
+      </c>
+      <c r="I234" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="235" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C235" t="s">
+        <v>66</v>
+      </c>
+      <c r="D235" t="s">
+        <v>193</v>
+      </c>
+      <c r="E235" t="s">
+        <v>64</v>
+      </c>
+      <c r="I235" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="236" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C236" t="s">
+        <v>66</v>
+      </c>
+      <c r="D236" t="s">
+        <v>195</v>
+      </c>
+      <c r="E236" t="s">
+        <v>64</v>
+      </c>
+      <c r="I236" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="237" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C237" t="s">
+        <v>66</v>
+      </c>
+      <c r="D237" t="s">
+        <v>197</v>
+      </c>
+      <c r="E237" t="s">
+        <v>64</v>
+      </c>
+      <c r="I237" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="238" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C238" t="s">
+        <v>66</v>
+      </c>
+      <c r="D238" t="s">
+        <v>199</v>
+      </c>
+      <c r="E238" t="s">
+        <v>64</v>
+      </c>
+      <c r="I238" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="239" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C239" t="s">
+        <v>66</v>
+      </c>
+      <c r="D239" t="s">
+        <v>201</v>
+      </c>
+      <c r="E239" t="s">
+        <v>64</v>
+      </c>
+      <c r="I239" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="240" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C240" t="s">
+        <v>66</v>
+      </c>
+      <c r="D240" t="s">
+        <v>203</v>
+      </c>
+      <c r="E240" t="s">
+        <v>64</v>
+      </c>
+      <c r="I240" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="241" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C241" t="s">
+        <v>66</v>
+      </c>
+      <c r="D241" t="s">
+        <v>205</v>
+      </c>
+      <c r="E241" t="s">
+        <v>64</v>
+      </c>
+      <c r="I241" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="242" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C242" t="s">
+        <v>66</v>
+      </c>
+      <c r="D242" t="s">
+        <v>207</v>
+      </c>
+      <c r="E242" t="s">
+        <v>64</v>
+      </c>
+      <c r="I242" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="243" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C243" t="s">
+        <v>66</v>
+      </c>
+      <c r="D243" t="s">
+        <v>209</v>
+      </c>
+      <c r="E243" t="s">
+        <v>64</v>
+      </c>
+      <c r="I243" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="244" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C244" t="s">
+        <v>66</v>
+      </c>
+      <c r="D244" t="s">
+        <v>211</v>
+      </c>
+      <c r="E244" t="s">
+        <v>64</v>
+      </c>
+      <c r="I244" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="245" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C245" t="s">
+        <v>66</v>
+      </c>
+      <c r="D245" t="s">
+        <v>213</v>
+      </c>
+      <c r="E245" t="s">
+        <v>64</v>
+      </c>
+      <c r="I245" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="246" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C246" t="s">
+        <v>66</v>
+      </c>
+      <c r="D246" t="s">
+        <v>215</v>
+      </c>
+      <c r="E246" t="s">
+        <v>64</v>
+      </c>
+      <c r="I246" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="247" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C247" t="s">
+        <v>66</v>
+      </c>
+      <c r="D247" t="s">
+        <v>217</v>
+      </c>
+      <c r="E247" t="s">
+        <v>64</v>
+      </c>
+      <c r="I247" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="248" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C248" t="s">
+        <v>66</v>
+      </c>
+      <c r="D248" t="s">
+        <v>219</v>
+      </c>
+      <c r="E248" t="s">
+        <v>64</v>
+      </c>
+      <c r="I248" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="249" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C249" t="s">
+        <v>66</v>
+      </c>
+      <c r="D249" t="s">
+        <v>221</v>
+      </c>
+      <c r="E249" t="s">
+        <v>64</v>
+      </c>
+      <c r="I249" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="250" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C250" t="s">
+        <v>66</v>
+      </c>
+      <c r="D250" t="s">
+        <v>223</v>
+      </c>
+      <c r="E250" t="s">
+        <v>64</v>
+      </c>
+      <c r="I250" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="251" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C251" t="s">
+        <v>66</v>
+      </c>
+      <c r="D251" t="s">
+        <v>225</v>
+      </c>
+      <c r="E251" t="s">
+        <v>64</v>
+      </c>
+      <c r="I251" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="252" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C252" t="s">
+        <v>66</v>
+      </c>
+      <c r="D252" t="s">
+        <v>227</v>
+      </c>
+      <c r="E252" t="s">
+        <v>64</v>
+      </c>
+      <c r="I252" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="253" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C253" t="s">
+        <v>66</v>
+      </c>
+      <c r="D253" t="s">
+        <v>229</v>
+      </c>
+      <c r="E253" t="s">
+        <v>64</v>
+      </c>
+      <c r="I253" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="254" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C254" t="s">
+        <v>66</v>
+      </c>
+      <c r="D254" t="s">
+        <v>231</v>
+      </c>
+      <c r="E254" t="s">
+        <v>64</v>
+      </c>
+      <c r="I254" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="255" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C255" t="s">
+        <v>66</v>
+      </c>
+      <c r="D255" t="s">
+        <v>233</v>
+      </c>
+      <c r="E255" t="s">
+        <v>64</v>
+      </c>
+      <c r="I255" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="256" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C256" t="s">
+        <v>66</v>
+      </c>
+      <c r="D256" t="s">
+        <v>235</v>
+      </c>
+      <c r="E256" t="s">
+        <v>64</v>
+      </c>
+      <c r="I256" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="257" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C257" t="s">
+        <v>66</v>
+      </c>
+      <c r="D257" t="s">
+        <v>237</v>
+      </c>
+      <c r="E257" t="s">
+        <v>64</v>
+      </c>
+      <c r="I257" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="258" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C258" t="s">
+        <v>66</v>
+      </c>
+      <c r="D258" t="s">
+        <v>239</v>
+      </c>
+      <c r="E258" t="s">
+        <v>64</v>
+      </c>
+      <c r="I258" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="259" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C259" t="s">
+        <v>66</v>
+      </c>
+      <c r="D259" t="s">
+        <v>241</v>
+      </c>
+      <c r="E259" t="s">
+        <v>64</v>
+      </c>
+      <c r="I259" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="260" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C260" t="s">
+        <v>66</v>
+      </c>
+      <c r="D260" t="s">
+        <v>243</v>
+      </c>
+      <c r="E260" t="s">
+        <v>64</v>
+      </c>
+      <c r="I260" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="261" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C261" t="s">
+        <v>66</v>
+      </c>
+      <c r="D261" t="s">
+        <v>245</v>
+      </c>
+      <c r="E261" t="s">
+        <v>64</v>
+      </c>
+      <c r="I261" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="262" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C262" t="s">
+        <v>66</v>
+      </c>
+      <c r="D262" t="s">
+        <v>247</v>
+      </c>
+      <c r="E262" t="s">
+        <v>64</v>
+      </c>
+      <c r="I262" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="263" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C263" t="s">
+        <v>66</v>
+      </c>
+      <c r="D263" t="s">
+        <v>249</v>
+      </c>
+      <c r="E263" t="s">
+        <v>64</v>
+      </c>
+      <c r="I263" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="264" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C264" t="s">
+        <v>66</v>
+      </c>
+      <c r="D264" t="s">
+        <v>251</v>
+      </c>
+      <c r="E264" t="s">
+        <v>64</v>
+      </c>
+      <c r="I264" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="265" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C265" t="s">
+        <v>66</v>
+      </c>
+      <c r="D265" t="s">
+        <v>253</v>
+      </c>
+      <c r="E265" t="s">
+        <v>64</v>
+      </c>
+      <c r="I265" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="266" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C266" t="s">
+        <v>66</v>
+      </c>
+      <c r="D266" t="s">
+        <v>255</v>
+      </c>
+      <c r="E266" t="s">
+        <v>64</v>
+      </c>
+      <c r="I266" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="267" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C267" t="s">
+        <v>66</v>
+      </c>
+      <c r="D267" t="s">
+        <v>257</v>
+      </c>
+      <c r="E267" t="s">
+        <v>64</v>
+      </c>
+      <c r="I267" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="268" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C268" t="s">
+        <v>66</v>
+      </c>
+      <c r="D268" t="s">
+        <v>259</v>
+      </c>
+      <c r="E268" t="s">
+        <v>64</v>
+      </c>
+      <c r="I268" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="269" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C269" t="s">
+        <v>66</v>
+      </c>
+      <c r="D269" t="s">
+        <v>261</v>
+      </c>
+      <c r="E269" t="s">
+        <v>64</v>
+      </c>
+      <c r="I269" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="270" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C270" t="s">
+        <v>66</v>
+      </c>
+      <c r="D270" t="s">
+        <v>263</v>
+      </c>
+      <c r="E270" t="s">
+        <v>64</v>
+      </c>
+      <c r="I270" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="271" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C271" t="s">
+        <v>66</v>
+      </c>
+      <c r="D271" t="s">
+        <v>265</v>
+      </c>
+      <c r="E271" t="s">
+        <v>64</v>
+      </c>
+      <c r="I271" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="272" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C272" t="s">
+        <v>66</v>
+      </c>
+      <c r="D272" t="s">
+        <v>267</v>
+      </c>
+      <c r="E272" t="s">
+        <v>64</v>
+      </c>
+      <c r="I272" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="273" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C273" t="s">
+        <v>66</v>
+      </c>
+      <c r="D273" t="s">
+        <v>269</v>
+      </c>
+      <c r="E273" t="s">
+        <v>57</v>
+      </c>
+      <c r="I273" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="274" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C274" t="s">
+        <v>66</v>
+      </c>
+      <c r="D274" t="s">
+        <v>271</v>
+      </c>
+      <c r="E274" t="s">
+        <v>57</v>
+      </c>
+      <c r="I274" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="275" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C275" t="s">
+        <v>66</v>
+      </c>
+      <c r="D275" t="s">
+        <v>273</v>
+      </c>
+      <c r="E275" t="s">
+        <v>57</v>
+      </c>
+      <c r="I275" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="276" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C276" t="s">
+        <v>66</v>
+      </c>
+      <c r="D276" t="s">
+        <v>275</v>
+      </c>
+      <c r="E276" t="s">
+        <v>57</v>
+      </c>
+      <c r="I276" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="277" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C277" t="s">
+        <v>66</v>
+      </c>
+      <c r="D277" t="s">
+        <v>277</v>
+      </c>
+      <c r="E277" t="s">
+        <v>57</v>
+      </c>
+      <c r="I277" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C278" t="s">
+        <v>66</v>
+      </c>
+      <c r="D278" t="s">
+        <v>279</v>
+      </c>
+      <c r="E278" t="s">
+        <v>57</v>
+      </c>
+      <c r="I278" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="279" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C279" t="s">
+        <v>66</v>
+      </c>
+      <c r="D279" t="s">
+        <v>281</v>
+      </c>
+      <c r="E279" t="s">
+        <v>57</v>
+      </c>
+      <c r="I279" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C280" t="s">
+        <v>66</v>
+      </c>
+      <c r="D280" t="s">
+        <v>283</v>
+      </c>
+      <c r="E280" t="s">
+        <v>57</v>
+      </c>
+      <c r="I280" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="281" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C281" t="s">
+        <v>66</v>
+      </c>
+      <c r="D281" t="s">
+        <v>285</v>
+      </c>
+      <c r="E281" t="s">
+        <v>286</v>
+      </c>
+      <c r="I281" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C282" t="s">
+        <v>66</v>
+      </c>
+      <c r="D282" t="s">
         <v>288</v>
       </c>
-      <c r="E224" t="s">
-        <v>64</v>
-      </c>
-      <c r="I224" t="s">
+      <c r="E282" t="s">
+        <v>64</v>
+      </c>
+      <c r="I282" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A225" t="s">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A283" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A226" t="s">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A284" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A227" t="s">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A285" t="s">
         <v>293</v>
       </c>
-      <c r="B227" t="s">
+      <c r="B285" t="s">
         <v>51</v>
       </c>
-      <c r="C227" t="b">
+      <c r="C285" t="b">
         <v>0</v>
       </c>
-      <c r="D227" t="s">
+      <c r="D285" t="s">
         <v>270</v>
       </c>
-      <c r="E227" t="s">
+      <c r="E285" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A228" t="s">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A286" t="s">
         <v>417</v>
       </c>
-      <c r="B228" t="s">
+      <c r="B286" t="s">
         <v>51</v>
       </c>
-      <c r="C228" t="b">
+      <c r="C286" t="b">
         <v>0</v>
       </c>
-      <c r="D228" t="s">
+      <c r="D286" t="s">
         <v>100</v>
       </c>
-      <c r="E228" t="s">
+      <c r="E286" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A229" t="s">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A287" t="s">
         <v>443</v>
       </c>
-      <c r="B229" t="s">
+      <c r="B287" t="s">
         <v>51</v>
       </c>
-      <c r="C229" t="b">
+      <c r="C287" t="b">
         <v>0</v>
       </c>
-      <c r="D229" t="s">
+      <c r="D287" t="s">
         <v>98</v>
       </c>
-      <c r="E229" t="s">
+      <c r="E287" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A230" t="s">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A288" t="s">
+        <v>479</v>
+      </c>
+      <c r="B288" t="s">
+        <v>51</v>
+      </c>
+      <c r="C288" t="b">
+        <v>0</v>
+      </c>
+      <c r="D288" t="s">
+        <v>276</v>
+      </c>
+      <c r="E288" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A289" t="s">
         <v>294</v>
       </c>
     </row>
@@ -5379,7 +5939,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
@@ -5778,9 +6338,43 @@
         <v>447</v>
       </c>
     </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>291</v>
+      </c>
+      <c r="B53" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>0</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>481</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A49:B48">
-    <sortCondition ref="A48"/>
+  <sortState ref="A54:B53">
+    <sortCondition ref="A53"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5832,4 +6426,125 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C6:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B1" t="s">
+        <v>449</v>
+      </c>
+      <c r="C1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D1" t="s">
+        <v>451</v>
+      </c>
+      <c r="E1" t="s">
+        <v>453</v>
+      </c>
+      <c r="F1" t="s">
+        <v>455</v>
+      </c>
+      <c r="G1" t="s">
+        <v>457</v>
+      </c>
+      <c r="H1" t="s">
+        <v>458</v>
+      </c>
+      <c r="I1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>482</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="4"/>
+      <c r="H2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>444</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="4"/>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="8">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Datatype Control" error="The column requires values of the int datatype." sqref="B2:B3">
+      <formula1>-2147483648</formula1>
+      <formula2>2147483647</formula2>
+    </dataValidation>
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Datatype Control" error="The column requires values of the varchar(50) datatype." sqref="C2:C3">
+      <formula1>50</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Datatype Control" error="The column requires values of the char(1) datatype." sqref="D2:D3">
+      <formula1>1</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Datatype Control" error="The column requires values of the datetime datatype." sqref="E2:E3">
+      <formula1>1</formula1>
+    </dataValidation>
+    <dataValidation type="time" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Datatype Control" error="The column requires values of the time datatype." sqref="F2:F3">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Datatype Control" error="The column requires values of the datetime datatype." sqref="G2:G3">
+      <formula1>1</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Datatype Control" error="The column requires values of the int datatype." sqref="H2:H3">
+      <formula1>-2147483648</formula1>
+      <formula2>2147483647</formula2>
+    </dataValidation>
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Datatype Control" error="The column requires values of the varchar(100) datatype." sqref="I2:I3">
+      <formula1>100</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>